<commit_message>
Adult norms through iwr
</commit_message>
<xml_diff>
--- a/OUTPUT-FILES/NORMS/TODC_adult_10.28.21_for norms/bln_sum-adult-raw-ss-lookup-tabbed-age.xlsx
+++ b/OUTPUT-FILES/NORMS/TODC_adult_10.28.21_for norms/bln_sum-adult-raw-ss-lookup-tabbed-age.xlsx
@@ -356,7 +356,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -376,7 +376,7 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>40</v>
@@ -384,7 +384,7 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>40</v>
@@ -392,7 +392,7 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>40</v>
@@ -400,7 +400,7 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>40</v>
@@ -408,7 +408,7 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>40</v>
@@ -416,7 +416,7 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>40</v>
@@ -424,186 +424,194 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
         <v>29</v>
       </c>
-      <c r="B30">
-        <v>127</v>
+      <c r="B31">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -613,7 +621,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -633,7 +641,7 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>40</v>
@@ -641,7 +649,7 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>40</v>
@@ -649,7 +657,7 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>40</v>
@@ -657,7 +665,7 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>40</v>
@@ -665,7 +673,7 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>40</v>
@@ -673,7 +681,7 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>40</v>
@@ -681,185 +689,193 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
         <v>29</v>
       </c>
-      <c r="B30">
+      <c r="B31">
         <v>123</v>
       </c>
     </row>
@@ -870,7 +886,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -890,7 +906,7 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>40</v>
@@ -898,7 +914,7 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>40</v>
@@ -906,7 +922,7 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>40</v>
@@ -914,7 +930,7 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>40</v>
@@ -922,7 +938,7 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>40</v>
@@ -930,194 +946,202 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
         <v>29</v>
       </c>
-      <c r="B30">
-        <v>120</v>
+      <c r="B31">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1127,7 +1151,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1147,7 +1171,7 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>40</v>
@@ -1155,7 +1179,7 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>40</v>
@@ -1163,7 +1187,7 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>40</v>
@@ -1171,7 +1195,7 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>40</v>
@@ -1179,7 +1203,7 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>40</v>
@@ -1187,193 +1211,201 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
         <v>29</v>
       </c>
-      <c r="B30">
+      <c r="B31">
         <v>121</v>
       </c>
     </row>
@@ -1384,7 +1416,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1404,7 +1436,7 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>40</v>
@@ -1412,7 +1444,7 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>40</v>
@@ -1420,7 +1452,7 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>40</v>
@@ -1428,7 +1460,7 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>40</v>
@@ -1436,202 +1468,210 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>93</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>117</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>120</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
         <v>29</v>
       </c>
-      <c r="B30">
-        <v>126</v>
+      <c r="B31">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1641,7 +1681,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1661,7 +1701,7 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>40</v>
@@ -1669,7 +1709,7 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>40</v>
@@ -1677,7 +1717,7 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>40</v>
@@ -1685,210 +1725,218 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>61</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>69</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>75</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>80</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>85</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>88</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>92</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>95</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>98</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>101</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>104</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>107</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>109</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>114</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>119</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>121</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>123</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>125</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>128</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>130</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>130</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>130</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>130</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
         <v>29</v>
       </c>
-      <c r="B30">
-        <v>130</v>
+      <c r="B31">
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>